<commit_message>
add remark to cal record
</commit_message>
<xml_diff>
--- a/doc/工作计划.xlsx
+++ b/doc/工作计划.xlsx
@@ -585,7 +585,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -609,9 +609,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -656,6 +653,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1855,88 +1858,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:8">
       <c r="B10" s="3" t="s">
@@ -2052,15 +2055,15 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="3" t="s">
@@ -2160,31 +2163,31 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2228,13 +2231,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2281,7 +2284,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2336,145 +2339,145 @@
       <c r="B2" s="9">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="30">
         <v>8</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="21" t="s">
+      <c r="G2" s="30"/>
+      <c r="H2" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:12">
       <c r="B3" s="9">
         <v>4.2</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="21" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:12">
       <c r="B4" s="9">
         <v>4.3</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="23" t="s">
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="I4" s="20"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" spans="1:12">
       <c r="B5" s="9">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="23" t="s">
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="I5" s="20"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" s="9">
         <v>4.5</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="23" t="s">
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="I6" s="20"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" s="9">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="23" t="s">
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:12">
       <c r="B8" s="9">
         <v>4.7</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="23" t="s">
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="I8" s="20"/>
-    </row>
-    <row r="9" spans="1:12" s="24" customFormat="1">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22" t="s">
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:12" s="23" customFormat="1">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22">
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21">
         <v>8</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22" t="s">
+      <c r="G9" s="21"/>
+      <c r="H9" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="I9" s="26"/>
-    </row>
-    <row r="10" spans="1:12" s="24" customFormat="1">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22" t="s">
+      <c r="I9" s="25"/>
+    </row>
+    <row r="10" spans="1:12" s="23" customFormat="1">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22">
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21">
         <v>6</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="21"/>
+      <c r="H10" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="I10" s="26"/>
-      <c r="K10" s="24" t="s">
+      <c r="I10" s="25"/>
+      <c r="K10" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="24" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2482,99 +2485,99 @@
       <c r="B11" s="9">
         <v>6.2</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="31" t="s">
         <v>83</v>
       </c>
       <c r="F11" s="9">
         <v>0.5</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I11" s="20"/>
+      <c r="I11" s="19"/>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" s="9">
         <v>6.3</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="31" t="s">
         <v>84</v>
       </c>
       <c r="F12" s="9">
         <v>1</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I12" s="20"/>
+      <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:12">
       <c r="B13" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="31" t="s">
         <v>86</v>
       </c>
       <c r="F13" s="9">
         <v>0.5</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I13" s="20"/>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:12">
       <c r="B14" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="31" t="s">
         <v>88</v>
       </c>
       <c r="F14" s="9">
         <v>1</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I14" s="20"/>
+      <c r="I14" s="19"/>
     </row>
     <row r="15" spans="1:12">
       <c r="B15" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="31" t="s">
         <v>91</v>
       </c>
       <c r="F15" s="9">
         <v>1.5</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I15" s="20"/>
-    </row>
-    <row r="16" spans="1:12" s="24" customFormat="1">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22" t="s">
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="1:12" s="23" customFormat="1">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22">
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21">
         <v>4</v>
       </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22" t="s">
+      <c r="G16" s="21"/>
+      <c r="H16" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="K16" s="24" t="s">
+      <c r="I16" s="25"/>
+      <c r="K16" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="L16" s="25" t="s">
+      <c r="L16" s="24" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2582,61 +2585,61 @@
       <c r="B17" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="31" t="s">
         <v>104</v>
       </c>
       <c r="F17" s="9">
         <v>0.5</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I17" s="20"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="2:12">
       <c r="B18" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="31" t="s">
         <v>105</v>
       </c>
       <c r="F18" s="9">
         <v>1</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I18" s="20"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="31" t="s">
         <v>106</v>
       </c>
       <c r="F19" s="9">
         <v>1.5</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I19" s="20"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" spans="2:12">
       <c r="B20" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="31" t="s">
         <v>107</v>
       </c>
       <c r="F20" s="9">
         <v>3</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I20" s="20"/>
+      <c r="I20" s="19"/>
       <c r="K20" t="s">
         <v>94</v>
       </c>
@@ -2648,76 +2651,76 @@
       <c r="B21" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="31" t="s">
         <v>109</v>
       </c>
       <c r="F21" s="9">
         <v>3</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I21" s="20"/>
+      <c r="I21" s="19"/>
     </row>
     <row r="22" spans="2:12">
       <c r="B22" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="31" t="s">
         <v>111</v>
       </c>
       <c r="F22" s="9">
         <v>1</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="H22" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I22" s="20"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="2:12">
       <c r="B23" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="31" t="s">
         <v>113</v>
       </c>
       <c r="F23" s="9">
         <v>5</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I23" s="20"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="2:12">
       <c r="B24" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="31" t="s">
         <v>115</v>
       </c>
       <c r="F24" s="9">
         <v>1</v>
       </c>
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I24" s="20"/>
+      <c r="I24" s="19"/>
     </row>
     <row r="25" spans="2:12">
       <c r="B25" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="31" t="s">
         <v>117</v>
       </c>
       <c r="F25" s="9">
         <v>4</v>
       </c>
-      <c r="H25" s="19" t="s">
+      <c r="H25" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I25" s="20"/>
+      <c r="I25" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L25"/>
@@ -2759,124 +2762,124 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="15" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="17">
         <v>16</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="15">
+      <c r="D13" s="17"/>
+      <c r="E13" s="14">
         <f>C13/8</f>
         <v>2</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <f>D13/8</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="17">
         <v>52</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>1</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="14">
         <f>C14/8</f>
         <v>6.5</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <f t="shared" ref="F14:F18" si="0">D14/8</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="17">
         <v>68</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="15">
+      <c r="D15" s="17"/>
+      <c r="E15" s="14">
         <f t="shared" ref="E15:E18" si="1">C15/8</f>
         <v>8.5</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="17">
         <v>52</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="15">
+      <c r="D16" s="17"/>
+      <c r="E16" s="14">
         <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="17">
         <v>188</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="17">
         <v>1</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="14">
         <f t="shared" si="1"/>
         <v>23.5</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>

</xml_diff>